<commit_message>
Working on manuscript figures
</commit_message>
<xml_diff>
--- a/for_manuscript/modellers.xlsx
+++ b/for_manuscript/modellers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MGierlinski/Work/Projects/NCCProt/for_manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D2B77DF-9B06-9044-8C26-73C066A32B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AE4DFC-3016-B64A-A292-43A6A912A700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="26820" windowHeight="16200" xr2:uid="{DECBADCE-2A2E-934F-A33F-9649AB08E070}"/>
+    <workbookView xWindow="38920" yWindow="3100" windowWidth="26820" windowHeight="16200" xr2:uid="{DECBADCE-2A2E-934F-A33F-9649AB08E070}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>gene_symbol</t>
   </si>
@@ -98,9 +98,6 @@
     <t>group</t>
   </si>
   <si>
-    <t>SWI/SNF complexes</t>
-  </si>
-  <si>
     <t>CHRAC15</t>
   </si>
   <si>
@@ -183,6 +180,12 @@
   </si>
   <si>
     <t>INO80/SWR complexes</t>
+  </si>
+  <si>
+    <t>SWI/SNF complexes BAF</t>
+  </si>
+  <si>
+    <t>SWI/SNF complexes pBAF</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128D0EDD-2958-8C42-8004-8F213BEA043D}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -566,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -574,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -582,7 +585,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -590,7 +593,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -598,7 +601,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -606,7 +609,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -614,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -622,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -630,7 +633,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -638,7 +641,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -646,7 +649,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -654,7 +657,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -662,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -670,7 +673,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -678,7 +681,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -686,215 +689,223 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
         <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
         <v>47</v>
       </c>
-      <c r="B44" t="s">
-        <v>48</v>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>